<commit_message>
Entrega final del TP3
</commit_message>
<xml_diff>
--- a/TP/TP3/Tablas/horas_trabajadas.xlsx
+++ b/TP/TP3/Tablas/horas_trabajadas.xlsx
@@ -467,10 +467,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>41.82269644994017</v>
+        <v>36.78127506014435</v>
       </c>
       <c r="C2" t="n">
-        <v>73.08669336538834</v>
+        <v>21.57993692716249</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -479,7 +479,7 @@
         <v>40</v>
       </c>
       <c r="F2" t="n">
-        <v>1047</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>